<commit_message>
Adjust input data and model
</commit_message>
<xml_diff>
--- a/data/01_test_cases/WB2/raw/scenario_data.xlsx
+++ b/data/01_test_cases/WB2/raw/scenario_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\sddip\data\01_test_cases\WB2\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA22482B-732E-44AA-A170-079E1A62B92F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62987AE3-B9EE-4906-B8CF-6A9F2ACD3926}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="3855" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4245" yWindow="3330" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>t</t>
   </si>
@@ -36,7 +36,10 @@
     <t>p</t>
   </si>
   <si>
-    <t>Pd</t>
+    <t>Pd1</t>
+  </si>
+  <si>
+    <t>Pd2</t>
   </si>
 </sst>
 </file>
@@ -354,15 +357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,8 +378,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -387,10 +393,13 @@
         <v>1</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -401,10 +410,13 @@
         <v>0.5</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -415,6 +427,9 @@
         <v>0.5</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>200</v>
       </c>
     </row>

</xml_diff>